<commit_message>
Added addTrack button and View Tracks in Albums
</commit_message>
<xml_diff>
--- a/wwwroot/reports/concerts/concerts.xlsx
+++ b/wwwroot/reports/concerts/concerts.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Исполнитель</t>
   </si>
@@ -45,19 +45,19 @@
     <t>Название тура</t>
   </si>
   <si>
-    <t>Меланхолия</t>
+    <t>Волшебство</t>
   </si>
   <si>
     <t>Название концерта</t>
   </si>
   <si>
-    <t>ЗАЛУПА</t>
+    <t>Театр имени Достоевского</t>
   </si>
   <si>
     <t>Дата</t>
   </si>
   <si>
-    <t>2024-05-29 00:40</t>
+    <t>2024-05-31 21:00</t>
   </si>
   <si>
     <t>Город</t>
@@ -66,25 +66,43 @@
     <t>Муром</t>
   </si>
   <si>
-    <t>Я ЧЕ ЕБУ ЧТОЛЬ</t>
+    <t>Milo Hall</t>
+  </si>
+  <si>
+    <t>2024-06-08 21:01</t>
   </si>
   <si>
     <t>Кулебаки</t>
   </si>
   <si>
+    <t>Supe Hall</t>
+  </si>
+  <si>
+    <t>2024-05-30 21:01</t>
+  </si>
+  <si>
+    <t>Вача</t>
+  </si>
+  <si>
+    <t>Концертный зал Мило</t>
+  </si>
+  <si>
+    <t>2024-06-04 21:09</t>
+  </si>
+  <si>
+    <t>Нижний Новгород</t>
+  </si>
+  <si>
     <t>Kai Angel</t>
   </si>
   <si>
-    <t>Кристаллические лярвы</t>
-  </si>
-  <si>
-    <t>ПИЗДА</t>
-  </si>
-  <si>
-    <t>2024-05-29 00:41</t>
-  </si>
-  <si>
-    <t>Вача</t>
+    <t>Russian Underground</t>
+  </si>
+  <si>
+    <t>2024-05-31 21:02</t>
+  </si>
+  <si>
+    <t>2024-06-02 21:02</t>
   </si>
 </sst>
 </file>
@@ -437,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DC5CD9-E6E2-4500-9E06-18E529AAF81F}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -500,49 +518,109 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="0" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>16</v>
+      <c r="F11" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>